<commit_message>
Update: Especiales y Expresiones invitadas
</commit_message>
<xml_diff>
--- a/data/propuestas_artisticas.xlsx
+++ b/data/propuestas_artisticas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7744" uniqueCount="2424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7744" uniqueCount="2425">
   <si>
     <t>Edad</t>
   </si>
@@ -7299,6 +7299,9 @@
   </si>
   <si>
     <t>DANZAS_REL</t>
+  </si>
+  <si>
+    <t>EXPRESIONES_I</t>
   </si>
 </sst>
 </file>
@@ -7781,11 +7784,13 @@
   <dimension ref="A1:AF314"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="5" max="5" width="65.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="36.7265625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8963,7 +8968,7 @@
         <v>33</v>
       </c>
       <c r="AF12" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -9551,7 +9556,7 @@
         <v>33</v>
       </c>
       <c r="AF18" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -9649,7 +9654,7 @@
         <v>33</v>
       </c>
       <c r="AF19" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -9747,7 +9752,7 @@
         <v>33</v>
       </c>
       <c r="AF20" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -11021,7 +11026,7 @@
         <v>33</v>
       </c>
       <c r="AF33" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -12099,7 +12104,7 @@
         <v>33</v>
       </c>
       <c r="AF44" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="45" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -12687,7 +12692,7 @@
         <v>33</v>
       </c>
       <c r="AF50" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="51" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -12785,7 +12790,7 @@
         <v>33</v>
       </c>
       <c r="AF51" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="52" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -12981,7 +12986,7 @@
         <v>33</v>
       </c>
       <c r="AF53" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="54" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -13961,7 +13966,7 @@
         <v>33</v>
       </c>
       <c r="AF63" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="64" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -14255,7 +14260,7 @@
         <v>33</v>
       </c>
       <c r="AF66" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="67" spans="1:32" ht="15" x14ac:dyDescent="0.35">
@@ -14745,7 +14750,7 @@
         <v>33</v>
       </c>
       <c r="AF71" s="14" t="s">
-        <v>2421</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="72" spans="1:32" ht="15" x14ac:dyDescent="0.35">

</xml_diff>